<commit_message>
Cập nhật link phân quyền
Cập nhật link phân quyền
</commit_message>
<xml_diff>
--- a/Kiểm tra phân quyền đăng nhập link.xlsx
+++ b/Kiểm tra phân quyền đăng nhập link.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB52E0D9-B96B-4539-A2DE-A78940E738E4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD474AF-D02E-4D74-BEDE-1DC8F6535617}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -449,7 +449,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -468,6 +467,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1116,7 +1116,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E83" sqref="E83"/>
+      <selection pane="bottomLeft" activeCell="B74" sqref="B74:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2455,39 +2455,39 @@
       <c r="A57" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
       <c r="G57" s="2"/>
     </row>
     <row r="58" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
       <c r="G59" s="2"/>
       <c r="H59" s="1" t="s">
         <v>19</v>
@@ -2566,13 +2566,13 @@
       <c r="A63" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B63" s="12" t="s">
+      <c r="B63" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
@@ -2627,41 +2627,41 @@
       <c r="A66" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B66" s="12" t="s">
+      <c r="B66" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B67" s="12" t="s">
+      <c r="B67" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B68" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>29</v>
+      <c r="B68" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>103</v>
@@ -2671,17 +2671,17 @@
       <c r="A69" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B69" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>29</v>
+      <c r="B69" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>103</v>
@@ -2691,17 +2691,17 @@
       <c r="A70" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B70" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>29</v>
+      <c r="B70" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E70" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>103</v>
@@ -2711,17 +2711,17 @@
       <c r="A71" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B71" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>29</v>
+      <c r="B71" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E71" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>103</v>
@@ -2731,17 +2731,17 @@
       <c r="A72" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B72" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E72" s="7" t="s">
-        <v>29</v>
+      <c r="B72" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E72" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>103</v>
@@ -2751,16 +2751,16 @@
       <c r="A73" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B73" s="15" t="s">
+      <c r="B73" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C73" s="15" t="s">
+      <c r="C73" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D73" s="15" t="s">
+      <c r="D73" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E73" s="15" t="s">
+      <c r="E73" s="14" t="s">
         <v>29</v>
       </c>
       <c r="F73" s="5" t="s">
@@ -2771,17 +2771,17 @@
       <c r="A74" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B74" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E74" s="7" t="s">
-        <v>29</v>
+      <c r="B74" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E74" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>103</v>
@@ -2797,10 +2797,10 @@
       <c r="C75" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="D75" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E75" s="9" t="s">
+      <c r="E75" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F75" s="5" t="s">
@@ -2811,16 +2811,16 @@
       <c r="A76" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B76" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C76" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D76" s="9" t="s">
+      <c r="C76" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E76" s="9" t="s">
+      <c r="E76" s="8" t="s">
         <v>103</v>
       </c>
       <c r="F76" s="5" t="s">
@@ -2831,16 +2831,16 @@
       <c r="A77" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B77" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C77" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D77" s="9" t="s">
+      <c r="D77" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="E77" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F77" s="5" t="s">
@@ -2851,16 +2851,16 @@
       <c r="A78" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C78" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D78" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E78" s="9" t="s">
+      <c r="E78" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F78" s="5" t="s">
@@ -2871,16 +2871,16 @@
       <c r="A79" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B79" s="15" t="s">
+      <c r="B79" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C79" s="15" t="s">
+      <c r="C79" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D79" s="15" t="s">
+      <c r="D79" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E79" s="15" t="s">
+      <c r="E79" s="14" t="s">
         <v>29</v>
       </c>
       <c r="F79" s="5" t="s">
@@ -2888,36 +2888,36 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="8" t="s">
+      <c r="A86" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B86" s="10" t="s">
+      <c r="B86" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="10"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="8" t="s">
+      <c r="A103" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B103" s="11" t="s">
+      <c r="B103" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="11"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="10"/>
+      <c r="F103" s="10"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="8" t="s">
+      <c r="A106" s="7" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="8" t="s">
+      <c r="A108" s="7" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>